<commit_message>
Implemented additional sophisticated effects block tests
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile2.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile2.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2964" windowWidth="31860" windowHeight="15060" activeTab="1"/>
+    <workbookView xWindow="2040" yWindow="2964" windowWidth="31860" windowHeight="15060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test conditions" sheetId="4" r:id="rId1"/>
     <sheet name="Test results" sheetId="5" r:id="rId2"/>
+    <sheet name="Test results 2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>Time points (hours - or specify any other units):</t>
   </si>
@@ -76,13 +77,46 @@
   </si>
   <si>
     <t>Replicate 3</t>
+  </si>
+  <si>
+    <t>Conc</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Eff1</t>
+  </si>
+  <si>
+    <t>Eff2</t>
+  </si>
+  <si>
+    <t>Eff3</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Quilifier</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>ErrQuil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,8 +195,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -223,6 +278,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -540,7 +612,7 @@
   <dimension ref="A1:AO10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,4 +1217,273 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="21">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21">
+        <v>2</v>
+      </c>
+      <c r="E1" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>0</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16">
+        <f>500 + 0.1*$A5 + 0.01*C$1</f>
+        <v>500.01</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" ref="D5:E9" si="0">500 + 0.1*$A5 + 0.01*D$1</f>
+        <v>500.02</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="0"/>
+        <v>500.03</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16">
+        <f>C5/20</f>
+        <v>25.000499999999999</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" ref="H5:I5" si="1">D5/20</f>
+        <v>25.000999999999998</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" si="1"/>
+        <v>25.0015</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="16">
+        <f t="shared" ref="C6:C9" si="2">500 + 0.1*$A6 + 0.01*C$1</f>
+        <v>500.11</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
+        <v>500.12</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>500.13</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16">
+        <f t="shared" ref="G6:G9" si="3">C6/20</f>
+        <v>25.005500000000001</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" ref="H6:H9" si="4">D6/20</f>
+        <v>25.006</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" ref="I6:I9" si="5">E6/20</f>
+        <v>25.006499999999999</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16">
+        <f t="shared" si="2"/>
+        <v>500.21</v>
+      </c>
+      <c r="D7" s="16">
+        <f t="shared" si="0"/>
+        <v>500.21999999999997</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>500.22999999999996</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <f t="shared" si="3"/>
+        <v>25.0105</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="4"/>
+        <v>25.010999999999999</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" si="5"/>
+        <v>25.011499999999998</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>3</v>
+      </c>
+      <c r="B8" s="16">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16">
+        <f t="shared" si="2"/>
+        <v>500.31</v>
+      </c>
+      <c r="D8" s="16">
+        <f t="shared" si="0"/>
+        <v>500.32</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>500.33</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16">
+        <f t="shared" si="3"/>
+        <v>25.015499999999999</v>
+      </c>
+      <c r="H8" s="16">
+        <f t="shared" si="4"/>
+        <v>25.015999999999998</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="5"/>
+        <v>25.016500000000001</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>4</v>
+      </c>
+      <c r="B9" s="16">
+        <v>25</v>
+      </c>
+      <c r="C9" s="16">
+        <f t="shared" si="2"/>
+        <v>500.40999999999997</v>
+      </c>
+      <c r="D9" s="16">
+        <f t="shared" si="0"/>
+        <v>500.41999999999996</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>500.42999999999995</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16">
+        <f t="shared" si="3"/>
+        <v>25.020499999999998</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" si="4"/>
+        <v>25.020999999999997</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="5"/>
+        <v>25.021499999999996</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>